<commit_message>
Inventario Paso 1 Ok
</commit_message>
<xml_diff>
--- a/AppComercial-Videos.xlsx
+++ b/AppComercial-Videos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppComercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EC22B8-8E1E-42BB-BBBA-599883C17CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91900AA5-B43D-41DD-87CF-F35618E73F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2304E8A-2790-4DC1-9361-D98A59767F40}"/>
   </bookViews>
@@ -861,7 +861,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
+      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>